<commit_message>
Database inputs feedback corrected and commented code deleted
</commit_message>
<xml_diff>
--- a/backend/v1.0/mockDB/Devices_test.xlsx
+++ b/backend/v1.0/mockDB/Devices_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Betan\Documents\GitHub\Microrred-USC\Tests\Digital_twins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\backend\v1.0\mockDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413C22BF-195D-496D-8F9B-8922488A3F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1364184-AFFF-4A4F-A4AB-223B18A4B55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro" sheetId="1" r:id="rId1"/>
@@ -727,7 +727,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
       </c>
       <c r="D11">
         <f>D13/D9</f>
-        <v>15</v>
+        <v>290.625</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -905,7 +905,7 @@
       </c>
       <c r="D12">
         <f>D13/D10</f>
-        <v>7.5</v>
+        <v>145.3125</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
       </c>
       <c r="D13">
         <f>D6*D7*0.75</f>
-        <v>600</v>
+        <v>11625</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -935,7 +935,7 @@
       </c>
       <c r="D14">
         <f>D6*D7*0.78</f>
-        <v>624</v>
+        <v>12090</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,7 +964,7 @@
       </c>
       <c r="D16">
         <f>D13*0.9/D15</f>
-        <v>21.513944223107568</v>
+        <v>416.83266932270914</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Querys from others biogasTKS for mass balance in biogas storage Systems
</commit_message>
<xml_diff>
--- a/backend/v1.0/mockDB/Devices_test.xlsx
+++ b/backend/v1.0/mockDB/Devices_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/mockDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C1364184-AFFF-4A4F-A4AB-223B18A4B55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85DBB843-D36F-42CE-A1A1-2863829D34BC}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{C1364184-AFFF-4A4F-A4AB-223B18A4B55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98AD5C41-89DB-4FDD-9E13-385DCF90CFB7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="233">
   <si>
     <t>Device</t>
   </si>
@@ -731,6 +731,12 @@
   </si>
   <si>
     <t>SV-109</t>
+  </si>
+  <si>
+    <t>Temperatura de biogás en V-102</t>
+  </si>
+  <si>
+    <t>TT-104</t>
   </si>
 </sst>
 </file>
@@ -795,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -803,6 +809,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1552,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C5547A-B804-42A6-8AAE-8D4287B541C3}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2012,7 +2019,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -2026,7 +2033,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -2040,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -2054,186 +2061,187 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>114</v>
       </c>
       <c r="B36" t="s">
+        <v>231</v>
+      </c>
+      <c r="C36" t="s">
+        <v>232</v>
+      </c>
+      <c r="D36">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
         <v>183</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>184</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
         <v>185</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>186</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" t="s">
         <v>187</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>188</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" t="s">
         <v>189</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>190</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" t="s">
         <v>191</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>192</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>114</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" t="s">
         <v>193</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>194</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" t="s">
         <v>195</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>196</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <v>500</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>114</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" t="s">
         <v>197</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>198</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" t="s">
         <v>199</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>200</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>1000</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>114</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" t="s">
         <v>201</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>202</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>114</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" t="s">
         <v>203</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>204</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>114</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" t="s">
         <v>205</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>206</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>114</v>
-      </c>
-      <c r="B48" t="s">
-        <v>207</v>
-      </c>
-      <c r="C48" t="s">
-        <v>208</v>
-      </c>
-      <c r="D48">
-        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2241,13 +2249,13 @@
         <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>207</v>
       </c>
       <c r="C49" t="s">
-        <v>116</v>
+        <v>208</v>
       </c>
       <c r="D49">
-        <v>2.4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -2255,13 +2263,13 @@
         <v>114</v>
       </c>
       <c r="B50" t="s">
-        <v>209</v>
+        <v>115</v>
       </c>
       <c r="C50" t="s">
-        <v>210</v>
+        <v>116</v>
       </c>
       <c r="D50">
-        <v>5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2269,13 +2277,13 @@
         <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C51" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D51">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2283,13 +2291,13 @@
         <v>114</v>
       </c>
       <c r="B52" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C52" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D52">
-        <v>2.4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2297,10 +2305,10 @@
         <v>114</v>
       </c>
       <c r="B53" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C53" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="D53">
         <v>2.4</v>
@@ -2311,13 +2319,13 @@
         <v>114</v>
       </c>
       <c r="B54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>160</v>
       </c>
       <c r="D54">
-        <v>5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -2325,13 +2333,13 @@
         <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C55" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D55">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2339,13 +2347,13 @@
         <v>114</v>
       </c>
       <c r="B56" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C56" t="s">
         <v>219</v>
       </c>
       <c r="D56">
-        <v>2.4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2353,10 +2361,10 @@
         <v>114</v>
       </c>
       <c r="B57" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="C57" t="s">
-        <v>186</v>
+        <v>219</v>
       </c>
       <c r="D57">
         <v>2.4</v>
@@ -2367,13 +2375,13 @@
         <v>114</v>
       </c>
       <c r="B58" t="s">
-        <v>221</v>
+        <v>185</v>
       </c>
       <c r="C58" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="D58">
-        <v>0.37</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2381,13 +2389,13 @@
         <v>114</v>
       </c>
       <c r="B59" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D59">
-        <v>0.5</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2395,13 +2403,13 @@
         <v>114</v>
       </c>
       <c r="B60" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C60" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2409,10 +2417,10 @@
         <v>114</v>
       </c>
       <c r="B61" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C61" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2423,17 +2431,32 @@
         <v>114</v>
       </c>
       <c r="B62" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C62" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
     </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" t="s">
+        <v>229</v>
+      </c>
+      <c r="C63" t="s">
+        <v>230</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solar model backend completed. Testing pending.
</commit_message>
<xml_diff>
--- a/backend/v1.0/mockDB/Devices_test.xlsx
+++ b/backend/v1.0/mockDB/Devices_test.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/mockDB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\backend\v1.0\mockDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{C1364184-AFFF-4A4F-A4AB-223B18A4B55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98AD5C41-89DB-4FDD-9E13-385DCF90CFB7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97521015-F954-4A1A-BD85-41222B9B240A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro" sheetId="1" r:id="rId1"/>
-    <sheet name="BiogasPlant" sheetId="3" r:id="rId2"/>
-    <sheet name="PV_WF" sheetId="2" r:id="rId3"/>
+    <sheet name="Hydro_depurado" sheetId="5" r:id="rId2"/>
+    <sheet name="BiogasPlant" sheetId="3" r:id="rId3"/>
+    <sheet name="PV_WF" sheetId="2" r:id="rId4"/>
+    <sheet name="PV_WF_depurado" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="243">
   <si>
     <t>Device</t>
   </si>
@@ -737,6 +739,36 @@
   </si>
   <si>
     <t>TT-104</t>
+  </si>
+  <si>
+    <t>Potencia de la carga DC del controlador (Controlador)</t>
+  </si>
+  <si>
+    <t>Temperatura de baterías (Controlador)</t>
+  </si>
+  <si>
+    <t>Voltaje de la red externa del inversor híbrido (inversor o analizador)</t>
+  </si>
+  <si>
+    <t>Voltaje de la carga DC del controlador (Controlador)</t>
+  </si>
+  <si>
+    <t>PDC001</t>
+  </si>
+  <si>
+    <t>TB001</t>
+  </si>
+  <si>
+    <t>PB001</t>
+  </si>
+  <si>
+    <t>VGR001</t>
+  </si>
+  <si>
+    <t>VDC001</t>
+  </si>
+  <si>
+    <t>Potencia DC de salida hacia las baterías (Controlador)</t>
   </si>
 </sst>
 </file>
@@ -801,7 +833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -809,7 +841,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,10 +858,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1100,14 +1129,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1121,7 +1150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1135,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1149,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1163,7 +1192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1177,7 +1206,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1191,7 +1220,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1205,7 +1234,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1219,7 +1248,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1234,7 +1263,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1248,7 +1277,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1263,7 +1292,7 @@
         <v>290.625</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1278,7 +1307,7 @@
         <v>145.3125</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1293,7 +1322,7 @@
         <v>11625</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1308,7 +1337,7 @@
         <v>12090</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1322,7 +1351,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -1337,7 +1366,7 @@
         <v>416.83266932270914</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1351,7 +1380,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1365,7 +1394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1379,7 +1408,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1394,7 +1423,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1408,7 +1437,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1422,7 +1451,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1437,7 +1466,7 @@
         <v>0.9797958971132712</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -1453,7 +1482,7 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
@@ -1467,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>53</v>
       </c>
@@ -1481,7 +1510,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>53</v>
       </c>
@@ -1495,7 +1524,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>53</v>
       </c>
@@ -1509,7 +1538,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
@@ -1523,7 +1552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>53</v>
       </c>
@@ -1537,7 +1566,7 @@
         <v>24.75</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>53</v>
       </c>
@@ -1558,20 +1587,484 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF1191F-099A-422D-901F-26AA5CD0988E}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11">
+        <f>D13/D9</f>
+        <v>290.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <f>D13/D10</f>
+        <v>145.3125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13">
+        <f>D6*D7*0.75</f>
+        <v>11625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14">
+        <f>D6*D7*0.78</f>
+        <v>12090</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <f>D13*0.9/D15</f>
+        <v>416.83266932270914</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2">
+        <f>D21/D19</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="4">
+        <f>D24/D21</f>
+        <v>0.9797958971132712</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="5">
+        <f>SQRT((D21*D21)-(D22*D22))</f>
+        <v>195.95917942265424</v>
+      </c>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="3">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="3">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="3">
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C5547A-B804-42A6-8AAE-8D4287B541C3}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +2078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -1599,7 +2092,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -1613,7 +2106,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -1627,7 +2120,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -1641,7 +2134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -1655,7 +2148,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -1669,7 +2162,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -1683,7 +2176,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -1697,7 +2190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -1711,7 +2204,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -1725,7 +2218,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -1739,7 +2232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -1753,7 +2246,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -1767,7 +2260,7 @@
         <v>40.479999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -1781,7 +2274,7 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -1795,7 +2288,7 @@
         <v>29.66</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -1809,7 +2302,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -1823,7 +2316,7 @@
         <v>0.21099999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -1837,7 +2330,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>114</v>
       </c>
@@ -1851,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -1865,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>114</v>
       </c>
@@ -1879,7 +2372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>114</v>
       </c>
@@ -1893,7 +2386,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>114</v>
       </c>
@@ -1907,7 +2400,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>114</v>
       </c>
@@ -1921,7 +2414,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>114</v>
       </c>
@@ -1935,7 +2428,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -1949,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -1963,7 +2456,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -1977,7 +2470,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -1991,7 +2484,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2005,7 +2498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -2019,7 +2512,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -2033,7 +2526,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -2047,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -2061,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -2075,7 +2568,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -2089,7 +2582,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>114</v>
       </c>
@@ -2102,9 +2595,8 @@
       <c r="D38">
         <v>2.4</v>
       </c>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -2118,7 +2610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -2132,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -2146,7 +2638,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -2160,7 +2652,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>114</v>
       </c>
@@ -2174,7 +2666,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>114</v>
       </c>
@@ -2188,7 +2680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -2202,7 +2694,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -2216,7 +2708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>114</v>
       </c>
@@ -2230,7 +2722,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>114</v>
       </c>
@@ -2244,7 +2736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>114</v>
       </c>
@@ -2258,7 +2750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>114</v>
       </c>
@@ -2272,7 +2764,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>114</v>
       </c>
@@ -2286,7 +2778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>114</v>
       </c>
@@ -2300,7 +2792,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>114</v>
       </c>
@@ -2314,7 +2806,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -2328,7 +2820,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>114</v>
       </c>
@@ -2342,7 +2834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>114</v>
       </c>
@@ -2356,7 +2848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -2370,7 +2862,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -2384,7 +2876,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -2398,7 +2890,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>114</v>
       </c>
@@ -2412,7 +2904,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -2426,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>114</v>
       </c>
@@ -2440,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -2460,22 +2952,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5844F91E-4DC3-4A3E-8A2D-69D108C045AE}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:D33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +2981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -2503,126 +2995,126 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D3">
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D6">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D7">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D8">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D9">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D10">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D11" s="4">
@@ -2630,42 +3122,42 @@
         <v>4.4444444444444446</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>54</v>
       </c>
       <c r="D12">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D14">
@@ -2673,126 +3165,126 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D15">
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D16">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D19">
         <v>13.6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D20">
         <v>13.9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="7" t="s">
         <v>50</v>
       </c>
       <c r="D21">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D22">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="4">
@@ -2800,42 +3292,42 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D24">
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D25">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="4">
@@ -2843,14 +3335,14 @@
         <v>0.9797958971132712</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="4">
@@ -2858,28 +3350,28 @@
         <v>195.95917942265424</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D28">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D29" s="4">
@@ -2887,42 +3379,42 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D30">
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D31">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="7" t="s">
         <v>96</v>
       </c>
       <c r="D32" s="4">
@@ -2930,14 +3422,14 @@
         <v>0.9797958971132712</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="3" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D33" s="4">
@@ -2945,78 +3437,409 @@
         <v>195.95917942265424</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="3" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="7" t="s">
         <v>111</v>
       </c>
       <c r="D34">
         <v>13.6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="7" t="s">
         <v>112</v>
       </c>
       <c r="D35">
         <v>13.9</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="3" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D36">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="3" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="7" t="s">
         <v>99</v>
       </c>
       <c r="D38">
         <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="D39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D42">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D43">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E441738-A19F-450F-8215-E106BB167EEB}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Solar backend offline and online tests
</commit_message>
<xml_diff>
--- a/backend/v1.0/mockDB/Devices_test.xlsx
+++ b/backend/v1.0/mockDB/Devices_test.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\backend\v1.0\mockDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973D8E35-2CAA-41E8-BFB3-0F4954429E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9AB559-89AC-4F85-8830-7A858ED7DEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro" sheetId="1" r:id="rId1"/>
-    <sheet name="Hydro_depurado" sheetId="5" r:id="rId2"/>
-    <sheet name="BiogasPlant" sheetId="3" r:id="rId3"/>
-    <sheet name="PV_WF" sheetId="2" r:id="rId4"/>
-    <sheet name="PV_WF_depurado" sheetId="4" r:id="rId5"/>
+    <sheet name="BiogasPlant" sheetId="3" r:id="rId2"/>
+    <sheet name="PV_WF" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="254">
   <si>
     <t>Device</t>
   </si>
@@ -96,21 +94,12 @@
     <t>PT002</t>
   </si>
   <si>
-    <t>Voltaje de las baterías (controladores de carga )</t>
-  </si>
-  <si>
     <t>VB001</t>
   </si>
   <si>
-    <t>Corriente de carga (controladores de carga )</t>
-  </si>
-  <si>
     <t>IC001</t>
   </si>
   <si>
-    <t>Temperatura Baterías (controladores de carga )</t>
-  </si>
-  <si>
     <t>TE003</t>
   </si>
   <si>
@@ -760,21 +749,6 @@
   </si>
   <si>
     <t>Potencia DC de salida hacia las baterías (Controlador)</t>
-  </si>
-  <si>
-    <t>Potencia de las baterías (controladores de carga )</t>
-  </si>
-  <si>
-    <t>Voltaje generada por turbina Pelton (controladores de carga )</t>
-  </si>
-  <si>
-    <t>Voltaje generada por turbina Turgo (controladores de carga )</t>
-  </si>
-  <si>
-    <t>Potencia generada por turbina Pelton (controladores de carga )</t>
-  </si>
-  <si>
-    <t>Potencia generada por turbina Turgo (controladores de carga )</t>
   </si>
   <si>
     <t>Voltaje generada por turbina Pelton (Controlador Pelton)</t>
@@ -835,7 +809,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -853,14 +827,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -892,15 +858,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,7 +1146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1209,502 +1172,502 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="5">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="D10">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11">
         <f>D13/D9</f>
         <v>290.625</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12">
         <f>D13/D10</f>
         <v>145.3125</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13">
         <f>D6*D7*0.75</f>
         <v>11625</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14">
         <f>D6*D7*0.78</f>
         <v>12090</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>244</v>
+      </c>
+      <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="5">
-        <v>25.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="D16">
         <f>D13*0.9/D15</f>
         <v>416.83266932270914</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>245</v>
+      </c>
+      <c r="C17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C19" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C20" t="s">
+        <v>252</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C21" t="s">
         <v>253</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="D17" s="5">
+      <c r="D21">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" s="5" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D19" s="5">
-        <v>25.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D20" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="D21" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="C24" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D24">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="C25" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="7">
+      <c r="D25" s="4">
         <f>D26/D24</f>
         <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="C28" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="6">
+      <c r="D28" s="2">
         <f>D29/D26</f>
         <v>0.9797958971132712</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="6">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="2">
         <f>SQRT((D26*D26)-(D27*D27))</f>
         <v>195.95917942265424</v>
       </c>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C33" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="D33">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="5">
-        <v>27.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="5">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="5">
+      <c r="D35">
         <v>24.75</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="5">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36">
         <v>1</v>
       </c>
     </row>
@@ -1715,204 +1678,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF1191F-099A-422D-901F-26AA5CD0988E}">
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>240</v>
-      </c>
-      <c r="C10" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C5547A-B804-42A6-8AAE-8D4287B541C3}">
   <dimension ref="A1:D63"/>
   <sheetViews>
@@ -1942,13 +1707,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D2">
         <v>2.4</v>
@@ -1956,13 +1721,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
         <v>111</v>
       </c>
-      <c r="B3" t="s">
-        <v>114</v>
-      </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D3">
         <v>35</v>
@@ -1970,13 +1735,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D4">
         <v>35</v>
@@ -1984,13 +1749,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -1998,13 +1763,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D6">
         <v>45</v>
@@ -2012,13 +1777,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -2026,13 +1791,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D8">
         <v>500</v>
@@ -2040,13 +1805,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -2054,13 +1819,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D10">
         <v>1000</v>
@@ -2068,13 +1833,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D11">
         <v>40</v>
@@ -2082,13 +1847,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -2096,13 +1861,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D13">
         <v>0.5</v>
@@ -2110,13 +1875,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D14">
         <v>40.479999999999997</v>
@@ -2124,13 +1889,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D15">
         <v>5.29</v>
@@ -2138,13 +1903,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D16">
         <v>29.66</v>
@@ -2152,13 +1917,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D17">
         <v>1.37</v>
@@ -2166,13 +1931,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D18">
         <v>0.21099999999999999</v>
@@ -2180,13 +1945,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D19">
         <v>1000</v>
@@ -2194,13 +1959,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2208,13 +1973,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2222,13 +1987,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D22">
         <v>30</v>
@@ -2236,13 +2001,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D23">
         <v>100</v>
@@ -2250,13 +2015,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D24">
         <v>2.4</v>
@@ -2264,13 +2029,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D25">
         <v>35</v>
@@ -2278,13 +2043,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D26">
         <v>35</v>
@@ -2292,13 +2057,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -2306,13 +2071,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D28">
         <v>45</v>
@@ -2320,13 +2085,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C29" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D29">
         <v>30</v>
@@ -2334,13 +2099,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D30">
         <v>500</v>
@@ -2348,13 +2113,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -2362,13 +2127,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C32" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D32">
         <v>1000</v>
@@ -2376,13 +2141,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D33">
         <v>40</v>
@@ -2390,13 +2155,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C34" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2404,13 +2169,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C35" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2418,13 +2183,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D36">
         <v>30</v>
@@ -2432,13 +2197,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D37">
         <v>100</v>
@@ -2446,13 +2211,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C38" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D38">
         <v>2.4</v>
@@ -2460,13 +2225,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C39" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D39">
         <v>30</v>
@@ -2474,13 +2239,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2488,13 +2253,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C41" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D41">
         <v>45</v>
@@ -2502,13 +2267,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C42" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D42">
         <v>30</v>
@@ -2516,13 +2281,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C43" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D43">
         <v>500</v>
@@ -2530,13 +2295,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C44" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D44">
         <v>5</v>
@@ -2544,13 +2309,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C45" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D45">
         <v>1000</v>
@@ -2558,13 +2323,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C46" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D46">
         <v>10</v>
@@ -2572,13 +2337,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C47" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D47">
         <v>30</v>
@@ -2586,13 +2351,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C48" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D48">
         <v>5</v>
@@ -2600,13 +2365,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B49" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D49">
         <v>10</v>
@@ -2614,13 +2379,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D50">
         <v>2.4</v>
@@ -2628,13 +2393,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C51" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D51">
         <v>5</v>
@@ -2642,13 +2407,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B52" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D52">
         <v>20</v>
@@ -2656,13 +2421,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C53" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D53">
         <v>2.4</v>
@@ -2670,13 +2435,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C54" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D54">
         <v>2.4</v>
@@ -2684,13 +2449,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D55">
         <v>5</v>
@@ -2698,13 +2463,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B56" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C56" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D56">
         <v>20</v>
@@ -2712,13 +2477,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B57" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C57" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D57">
         <v>2.4</v>
@@ -2726,13 +2491,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B58" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C58" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D58">
         <v>2.4</v>
@@ -2740,13 +2505,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C59" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D59">
         <v>0.37</v>
@@ -2754,13 +2519,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C60" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D60">
         <v>0.5</v>
@@ -2768,13 +2533,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B61" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C61" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2782,13 +2547,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B62" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C62" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2796,13 +2561,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B63" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C63" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2814,12 +2579,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5844F91E-4DC3-4A3E-8A2D-69D108C045AE}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2845,13 +2610,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>800</v>
@@ -2859,13 +2624,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3">
         <v>800</v>
@@ -2873,13 +2638,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -2887,13 +2652,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>100</v>
@@ -2901,10 +2666,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -2915,10 +2680,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -2929,13 +2694,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>46</v>
@@ -2943,13 +2708,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9">
         <v>47</v>
@@ -2957,13 +2722,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>18</v>
@@ -2971,13 +2736,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" s="2">
         <f>D12/D10</f>
@@ -2986,13 +2751,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>80</v>
@@ -3000,13 +2765,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -3014,13 +2779,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D14">
         <f>D15/D13</f>
@@ -3029,13 +2794,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D15">
         <v>180</v>
@@ -3043,13 +2808,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>13</v>
@@ -3057,13 +2822,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -3071,13 +2836,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3085,13 +2850,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D19">
         <v>13.6</v>
@@ -3099,13 +2864,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>13.9</v>
@@ -3113,13 +2878,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21">
         <v>12</v>
@@ -3127,13 +2892,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <v>120</v>
@@ -3141,13 +2906,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23" s="2">
         <f>D24/D22</f>
@@ -3156,13 +2921,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D24">
         <v>200</v>
@@ -3170,13 +2935,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D25">
         <v>40</v>
@@ -3184,13 +2949,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2">
         <f>D27/D24</f>
@@ -3199,13 +2964,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D27" s="2">
         <f>SQRT((D24*D24)-(D25*D25))</f>
@@ -3214,13 +2979,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <v>120</v>
@@ -3228,13 +2993,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D29" s="2">
         <f>D30/D28</f>
@@ -3243,13 +3008,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D30">
         <v>200</v>
@@ -3257,13 +3022,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D31">
         <v>40</v>
@@ -3271,13 +3036,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D32" s="2">
         <f>D33/D30</f>
@@ -3286,13 +3051,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
         <v>94</v>
-      </c>
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" t="s">
-        <v>97</v>
       </c>
       <c r="D33" s="2">
         <f>SQRT((D30*D30)-(D31*D31))</f>
@@ -3301,13 +3066,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D34">
         <v>13.6</v>
@@ -3315,13 +3080,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D35">
         <v>13.9</v>
@@ -3329,13 +3094,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D36">
         <v>12</v>
@@ -3343,13 +3108,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3357,13 +3122,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3371,13 +3136,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D39">
         <v>50</v>
@@ -3385,13 +3150,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C40" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D40">
         <v>12</v>
@@ -3399,13 +3164,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C41" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D41">
         <v>30</v>
@@ -3413,13 +3178,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C42" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D42">
         <v>150</v>
@@ -3427,13 +3192,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C43" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D43">
         <v>120</v>
@@ -3443,265 +3208,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E441738-A19F-450F-8215-E106BB167EEB}">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" t="s">
-        <v>230</v>
-      </c>
-      <c r="C18" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" t="s">
-        <v>233</v>
-      </c>
-      <c r="C19" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" t="s">
-        <v>231</v>
-      </c>
-      <c r="C20" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" t="s">
-        <v>239</v>
-      </c>
-      <c r="C21" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" t="s">
-        <v>232</v>
-      </c>
-      <c r="C22" t="s">
-        <v>237</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Turbine and solar updates
</commit_message>
<xml_diff>
--- a/backend/v1.0/mockDB/Devices_test.xlsx
+++ b/backend/v1.0/mockDB/Devices_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\backend\v1.0\mockDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\project-cali\backend\v1.0\mockDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9AB559-89AC-4F85-8830-7A858ED7DEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D3E918-1B14-4515-B4BE-5E9D26F7D6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="264">
   <si>
     <t>Device</t>
   </si>
@@ -247,9 +247,6 @@
     <t>Voltaje aerogenerador (fan) (Controlador)</t>
   </si>
   <si>
-    <t>VG005</t>
-  </si>
-  <si>
     <t>Corriente Aerogenerador (fan) (Controlador)</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>Potencia aerogenerador (fan)(Controlador)</t>
   </si>
   <si>
-    <t>PG005</t>
-  </si>
-  <si>
     <t>Voltaje de las baterías (Controlador)</t>
   </si>
   <si>
@@ -800,6 +794,42 @@
   </si>
   <si>
     <t>PB002</t>
+  </si>
+  <si>
+    <t>Voltaje de las baterías inversor híbrido</t>
+  </si>
+  <si>
+    <t>Temperatura de baterías inversor híbrido</t>
+  </si>
+  <si>
+    <t>TB002</t>
+  </si>
+  <si>
+    <t>Potencia paneles inversor híbrido</t>
+  </si>
+  <si>
+    <t>PG003</t>
+  </si>
+  <si>
+    <t>Potencia aerogenerador inversor híbrido</t>
+  </si>
+  <si>
+    <t>PG004</t>
+  </si>
+  <si>
+    <t>Potencia DC de salida hacia las baterías inversor híbrido</t>
+  </si>
+  <si>
+    <t>Voltaje Paneles solares inversor híbrido</t>
+  </si>
+  <si>
+    <t>VG003</t>
+  </si>
+  <si>
+    <t>Voltaje aerogenerador inversor híbrido</t>
+  </si>
+  <si>
+    <t>VG004</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1274,7 +1304,7 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C9" t="s">
         <v>50</v>
@@ -1289,7 +1319,7 @@
         <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
@@ -1303,7 +1333,7 @@
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C11" t="s">
         <v>49</v>
@@ -1318,7 +1348,7 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
@@ -1333,7 +1363,7 @@
         <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C13" t="s">
         <v>48</v>
@@ -1348,7 +1378,7 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C14" t="s">
         <v>55</v>
@@ -1363,7 +1393,7 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1377,7 +1407,7 @@
         <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -1392,10 +1422,10 @@
         <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D17">
         <v>100</v>
@@ -1406,7 +1436,7 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
@@ -1420,10 +1450,10 @@
         <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D19">
         <v>25.1</v>
@@ -1434,10 +1464,10 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1448,10 +1478,10 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D21">
         <v>100</v>
@@ -1462,10 +1492,10 @@
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22">
         <v>30</v>
@@ -1707,13 +1737,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
       </c>
       <c r="D2">
         <v>2.4</v>
@@ -1721,13 +1751,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3">
         <v>35</v>
@@ -1735,13 +1765,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D4">
         <v>35</v>
@@ -1749,13 +1779,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -1763,13 +1793,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6">
         <v>45</v>
@@ -1777,13 +1807,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -1791,13 +1821,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D8">
         <v>500</v>
@@ -1805,13 +1835,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -1819,13 +1849,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D10">
         <v>1000</v>
@@ -1833,13 +1863,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D11">
         <v>40</v>
@@ -1847,13 +1877,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -1861,13 +1891,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D13">
         <v>0.5</v>
@@ -1875,13 +1905,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D14">
         <v>40.479999999999997</v>
@@ -1889,13 +1919,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D15">
         <v>5.29</v>
@@ -1903,13 +1933,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D16">
         <v>29.66</v>
@@ -1917,13 +1947,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D17">
         <v>1.37</v>
@@ -1931,13 +1961,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D18">
         <v>0.21099999999999999</v>
@@ -1945,13 +1975,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D19">
         <v>1000</v>
@@ -1959,13 +1989,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1973,13 +2003,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1987,13 +2017,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D22">
         <v>30</v>
@@ -2001,13 +2031,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D23">
         <v>100</v>
@@ -2015,13 +2045,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D24">
         <v>2.4</v>
@@ -2029,13 +2059,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D25">
         <v>35</v>
@@ -2043,13 +2073,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26">
         <v>35</v>
@@ -2057,13 +2087,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -2071,13 +2101,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D28">
         <v>45</v>
@@ -2085,13 +2115,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D29">
         <v>30</v>
@@ -2099,13 +2129,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D30">
         <v>500</v>
@@ -2113,13 +2143,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -2127,13 +2157,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D32">
         <v>1000</v>
@@ -2141,13 +2171,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D33">
         <v>40</v>
@@ -2155,13 +2185,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2169,13 +2199,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2183,13 +2213,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D36">
         <v>30</v>
@@ -2197,13 +2227,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D37">
         <v>100</v>
@@ -2211,13 +2241,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D38">
         <v>2.4</v>
@@ -2225,13 +2255,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D39">
         <v>30</v>
@@ -2239,13 +2269,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2253,13 +2283,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C41" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D41">
         <v>45</v>
@@ -2267,13 +2297,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C42" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D42">
         <v>30</v>
@@ -2281,13 +2311,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D43">
         <v>500</v>
@@ -2295,13 +2325,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C44" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D44">
         <v>5</v>
@@ -2309,13 +2339,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D45">
         <v>1000</v>
@@ -2323,13 +2353,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D46">
         <v>10</v>
@@ -2337,13 +2367,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C47" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D47">
         <v>30</v>
@@ -2351,13 +2381,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D48">
         <v>5</v>
@@ -2365,13 +2395,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D49">
         <v>10</v>
@@ -2379,13 +2409,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" t="s">
         <v>108</v>
-      </c>
-      <c r="B50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C50" t="s">
-        <v>110</v>
       </c>
       <c r="D50">
         <v>2.4</v>
@@ -2393,13 +2423,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C51" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D51">
         <v>5</v>
@@ -2407,13 +2437,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C52" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D52">
         <v>20</v>
@@ -2421,13 +2451,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C53" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D53">
         <v>2.4</v>
@@ -2435,13 +2465,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D54">
         <v>2.4</v>
@@ -2449,13 +2479,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B55" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D55">
         <v>5</v>
@@ -2463,13 +2493,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B56" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C56" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D56">
         <v>20</v>
@@ -2477,13 +2507,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B57" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C57" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D57">
         <v>2.4</v>
@@ -2491,13 +2521,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C58" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D58">
         <v>2.4</v>
@@ -2505,13 +2535,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C59" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D59">
         <v>0.37</v>
@@ -2519,13 +2549,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C60" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D60">
         <v>0.5</v>
@@ -2533,13 +2563,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C61" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2547,13 +2577,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B62" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C62" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2561,13 +2591,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C63" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2581,10 +2611,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5844F91E-4DC3-4A3E-8A2D-69D108C045AE}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,7 +2640,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
@@ -2624,7 +2654,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -2638,7 +2668,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
@@ -2652,7 +2682,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
@@ -2666,7 +2696,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
@@ -2680,7 +2710,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
         <v>64</v>
@@ -2694,7 +2724,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
         <v>64</v>
@@ -2708,13 +2738,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
         <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D9">
         <v>47</v>
@@ -2722,7 +2752,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
         <v>65</v>
@@ -2736,7 +2766,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
         <v>66</v>
@@ -2751,7 +2781,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>67</v>
@@ -2765,13 +2795,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
         <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -2779,13 +2809,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
         <v>70</v>
-      </c>
-      <c r="C14" t="s">
-        <v>71</v>
       </c>
       <c r="D14">
         <f>D15/D13</f>
@@ -2794,13 +2824,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>180</v>
@@ -2808,10 +2838,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -2822,10 +2852,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
@@ -2836,13 +2866,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2850,10 +2880,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
         <v>42</v>
@@ -2864,10 +2894,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
@@ -2878,10 +2908,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -2892,7 +2922,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -2906,7 +2936,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
@@ -2921,10 +2951,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -2935,10 +2965,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
@@ -2949,10 +2979,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
@@ -2964,10 +2994,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
         <v>40</v>
@@ -2979,13 +3009,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28">
         <v>120</v>
@@ -2993,13 +3023,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2">
         <f>D30/D28</f>
@@ -3008,13 +3038,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D30">
         <v>200</v>
@@ -3022,13 +3052,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D31">
         <v>40</v>
@@ -3036,13 +3066,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D32" s="2">
         <f>D33/D30</f>
@@ -3051,13 +3081,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D33" s="2">
         <f>SQRT((D30*D30)-(D31*D31))</f>
@@ -3066,69 +3096,69 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>252</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="D34">
-        <v>13.6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D35">
-        <v>13.9</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D36">
-        <v>12</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3136,72 +3166,170 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" t="s">
         <v>91</v>
       </c>
-      <c r="B39" t="s">
-        <v>227</v>
-      </c>
-      <c r="C39" t="s">
-        <v>231</v>
-      </c>
       <c r="D39">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D40">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
         <v>228</v>
       </c>
       <c r="C41" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D41">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C42" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D42">
-        <v>150</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="C43" t="s">
+        <v>254</v>
+      </c>
+      <c r="D43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
         <v>234</v>
       </c>
-      <c r="D43">
+      <c r="C44" t="s">
+        <v>231</v>
+      </c>
+      <c r="D44">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>227</v>
+      </c>
+      <c r="C45" t="s">
+        <v>232</v>
+      </c>
+      <c r="D45">
         <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
+        <v>255</v>
+      </c>
+      <c r="C46" t="s">
+        <v>256</v>
+      </c>
+      <c r="D46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" t="s">
+        <v>257</v>
+      </c>
+      <c r="C47" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" t="s">
+        <v>259</v>
+      </c>
+      <c r="C48" t="s">
+        <v>251</v>
+      </c>
+      <c r="D48">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" t="s">
+        <v>260</v>
+      </c>
+      <c r="C49" t="s">
+        <v>261</v>
+      </c>
+      <c r="D49">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" t="s">
+        <v>262</v>
+      </c>
+      <c r="C50" t="s">
+        <v>263</v>
+      </c>
+      <c r="D50">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>